<commit_message>
Add native and contaminated strains to mock for challenging ROC
Changes to be committed:
	modified:   recentrifuge/__init__.py
	modified:   recentrifuge/test/TEST.rcf.html
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
	modified:   retest
	modified:   setup.py
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijm/local/recentrifuge/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijm/local/recentrifuge/recentrifuge/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="22060" windowWidth="26340" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="22060" windowWidth="26340" windowHeight="16960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>(float)</t>
+  </si>
+  <si>
+    <t>Methanobacterium formicicum DSM 3637</t>
+  </si>
+  <si>
+    <t>Methanobacterium formicicum JCM 10132</t>
   </si>
 </sst>
 </file>
@@ -326,8 +332,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -370,9 +380,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -648,13 +662,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -694,25 +710,25 @@
         <v>9606</v>
       </c>
       <c r="C2">
-        <v>87130</v>
+        <v>86830</v>
       </c>
       <c r="D2">
-        <v>60576</v>
+        <v>60573</v>
       </c>
       <c r="E2">
-        <v>87130</v>
+        <v>87100</v>
       </c>
       <c r="F2">
-        <v>34171</v>
+        <v>31168</v>
       </c>
       <c r="G2">
-        <v>28324</v>
+        <v>27994</v>
       </c>
       <c r="H2">
-        <v>18270</v>
+        <v>17940</v>
       </c>
       <c r="I2">
-        <v>20396</v>
+        <v>17393</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1181,97 +1197,97 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19">
+        <v>1204725</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <v>300</v>
+      </c>
+      <c r="I19">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20">
+        <v>1300163</v>
+      </c>
+      <c r="C20">
+        <v>300</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <v>3000</v>
+      </c>
+      <c r="G20">
+        <v>300</v>
+      </c>
+      <c r="H20">
+        <v>30</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>31998</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>5</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>5</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>5</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>398578</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>5000</v>
-      </c>
-      <c r="I20">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>80865</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>10000</v>
-      </c>
-      <c r="I21">
-        <v>5000</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22">
-        <v>80864</v>
+        <v>398578</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1289,70 +1305,128 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="I22">
         <v>5000</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>31</v>
+      <c r="A23" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>80865</v>
       </c>
       <c r="C23">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>10000</v>
       </c>
       <c r="I23">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>80864</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>10000</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="I24">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>10000</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25">
+        <v>10000</v>
+      </c>
+      <c r="F25">
+        <v>10000</v>
+      </c>
+      <c r="G25">
+        <v>10000</v>
+      </c>
+      <c r="H25">
+        <v>10000</v>
+      </c>
+      <c r="I25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C24">
-        <f t="shared" ref="C24:I24" si="0">SUM(C2:C23)</f>
+      <c r="C26">
+        <f t="shared" ref="C26:I26" si="0">SUM(C2:C25)</f>
         <v>100000</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="F24">
+      <c r="F26">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="G24">
+      <c r="G26">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="H24">
+      <c r="H26">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="I24">
+      <c r="I26">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>

</xml_diff>

<commit_message>
Improve testing: plot mintaxa, add ctrl statistical noise, and more
On branch master
	modified:   recentrifuge/__init__.py
	modified:   recentrifuge/test/TEST.rcf.html
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
	modified:   retest
	modified:   setup.py
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="22060" windowWidth="26340" windowHeight="16960" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="22060" windowWidth="27740" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Methanobacterium formicicum JCM 10132</t>
+  </si>
+  <si>
+    <t>statistical noise in negative control samples</t>
   </si>
 </sst>
 </file>
@@ -323,12 +326,107 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -341,7 +439,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -379,6 +477,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -664,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,25 +818,25 @@
         <v>9606</v>
       </c>
       <c r="C2">
-        <v>86830</v>
+        <v>86818</v>
       </c>
       <c r="D2">
-        <v>60573</v>
+        <v>60565</v>
       </c>
       <c r="E2">
-        <v>87100</v>
+        <v>87094</v>
       </c>
       <c r="F2">
-        <v>31168</v>
+        <v>33271</v>
       </c>
       <c r="G2">
-        <v>27994</v>
+        <v>28225</v>
       </c>
       <c r="H2">
-        <v>17940</v>
+        <v>18171</v>
       </c>
       <c r="I2">
-        <v>17393</v>
+        <v>19496</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1028,14 +1136,14 @@
       <c r="B13">
         <v>1587</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
+      <c r="C13" s="23">
+        <v>3</v>
+      </c>
+      <c r="D13" s="24">
+        <v>2</v>
+      </c>
+      <c r="E13" s="25">
+        <v>3</v>
       </c>
       <c r="F13">
         <v>6000</v>
@@ -1057,14 +1165,14 @@
       <c r="B14">
         <v>187218</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+      <c r="C14" s="26">
+        <v>1</v>
+      </c>
+      <c r="D14" s="27">
+        <v>0</v>
+      </c>
+      <c r="E14" s="28">
+        <v>1</v>
       </c>
       <c r="F14">
         <v>4260</v>
@@ -1086,14 +1194,14 @@
       <c r="B15">
         <v>1540099</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
+      <c r="C15" s="26">
+        <v>3</v>
+      </c>
+      <c r="D15" s="27">
+        <v>1</v>
+      </c>
+      <c r="E15" s="28">
+        <v>2</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1115,14 +1223,14 @@
       <c r="B16">
         <v>28901</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
+      <c r="C16" s="26">
+        <v>3</v>
+      </c>
+      <c r="D16" s="27">
+        <v>2</v>
+      </c>
+      <c r="E16" s="28">
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1144,13 +1252,13 @@
       <c r="B17">
         <v>54736</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
+      <c r="C17" s="26">
+        <v>0</v>
+      </c>
+      <c r="D17" s="27">
+        <v>1</v>
+      </c>
+      <c r="E17" s="28">
         <v>0</v>
       </c>
       <c r="F17">
@@ -1173,14 +1281,14 @@
       <c r="B18">
         <v>59201</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
+      <c r="C18" s="26">
+        <v>1</v>
+      </c>
+      <c r="D18" s="27">
+        <v>0</v>
+      </c>
+      <c r="E18" s="28">
+        <v>2</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1202,26 +1310,26 @@
       <c r="B19">
         <v>1204725</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
+      <c r="C19" s="29">
+        <v>1</v>
+      </c>
+      <c r="D19" s="30">
+        <v>2</v>
+      </c>
+      <c r="E19" s="31">
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="H19">
-        <v>300</v>
+        <v>90</v>
       </c>
       <c r="I19">
-        <v>3000</v>
+        <v>900</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1241,16 +1349,16 @@
         <v>30</v>
       </c>
       <c r="F20">
-        <v>3000</v>
+        <v>900</v>
       </c>
       <c r="G20">
-        <v>300</v>
+        <v>90</v>
       </c>
       <c r="H20">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1442,7 +1550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1519,7 +1629,12 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="32"/>
+      <c r="D12" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="21" t="s">

</xml_diff>

<commit_message>
Improve variable mintaxa test
On branch master
	modified:   recentrifuge/test/TEST.rcf.html
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
	modified:   retest
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="440" yWindow="22060" windowWidth="27740" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="820" yWindow="22080" windowWidth="26340" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -45,15 +45,9 @@
     <t>Triticum aestivum</t>
   </si>
   <si>
-    <t>Malassezia globosa CBS 7966</t>
-  </si>
-  <si>
     <t>Pan troglodytes</t>
   </si>
   <si>
-    <t>Propionibacterium phage SKKY</t>
-  </si>
-  <si>
     <t>Methanosarcina mazei</t>
   </si>
   <si>
@@ -190,6 +184,12 @@
   </si>
   <si>
     <t>statistical noise in negative control samples</t>
+  </si>
+  <si>
+    <t>Malassezia globosa</t>
+  </si>
+  <si>
+    <t>Propionibacterium virus SKKY</t>
   </si>
 </sst>
 </file>
@@ -430,8 +430,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -488,13 +490,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -773,7 +777,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,31 +787,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -818,13 +822,13 @@
         <v>9606</v>
       </c>
       <c r="C2">
-        <v>86818</v>
+        <v>86798</v>
       </c>
       <c r="D2">
-        <v>60565</v>
+        <v>60745</v>
       </c>
       <c r="E2">
-        <v>87094</v>
+        <v>88074</v>
       </c>
       <c r="F2">
         <v>33271</v>
@@ -870,7 +874,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>9598</v>
@@ -986,19 +990,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B8">
-        <v>425265</v>
+        <v>76773</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="F8">
         <v>5000</v>
@@ -1015,10 +1019,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B9">
-        <v>1655020</v>
+        <v>1982305</v>
       </c>
       <c r="C9">
         <v>500</v>
@@ -1044,7 +1048,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>2209</v>
@@ -1073,7 +1077,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>2208</v>
@@ -1102,7 +1106,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>1578</v>
@@ -1131,7 +1135,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>1587</v>
@@ -1160,7 +1164,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>187218</v>
@@ -1189,7 +1193,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>1540099</v>
@@ -1218,7 +1222,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>28901</v>
@@ -1247,7 +1251,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>54736</v>
@@ -1276,7 +1280,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>59201</v>
@@ -1305,7 +1309,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>1204725</v>
@@ -1334,7 +1338,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20">
         <v>1300163</v>
@@ -1363,7 +1367,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>31998</v>
@@ -1392,7 +1396,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>398578</v>
@@ -1421,7 +1425,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>80865</v>
@@ -1450,7 +1454,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>80864</v>
@@ -1479,7 +1483,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1508,7 +1512,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <f t="shared" ref="C26:I26" si="0">SUM(C2:C25)</f>
@@ -1564,81 +1568,81 @@
     <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="32"/>
       <c r="D12" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1646,11 +1650,11 @@
     </row>
     <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E16" s="22">
         <v>0.01</v>
@@ -1658,11 +1662,11 @@
     </row>
     <row r="17" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E17" s="22">
         <v>1E-3</v>

</xml_diff>

<commit_message>
Improve scalability of testing by moving data to sheet on mock.xlsx
On branch master
	modified:   recentrifuge/__init__.py
	modified:   recentrifuge/config.py
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
	modified:   retest
	modified:   setup.py
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="22080" windowWidth="26340" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="2200" yWindow="1560" windowWidth="31460" windowHeight="19500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
-    <sheet name="types" sheetId="2" r:id="rId2"/>
+    <sheet name="key" sheetId="3" r:id="rId2"/>
+    <sheet name="types" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -190,6 +191,168 @@
   </si>
   <si>
     <t>Propionibacterium virus SKKY</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>HATCH</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>RANK</t>
+  </si>
+  <si>
+    <t>"x"</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>"\\"</t>
+  </si>
+  <si>
+    <t>["smpl3", "smpl4"]</t>
+  </si>
+  <si>
+    <t>no_rank_species</t>
+  </si>
+  <si>
+    <t>"O"</t>
+  </si>
+  <si>
+    <t>["smpl2", "smpl4"]</t>
+  </si>
+  <si>
+    <t>"//"</t>
+  </si>
+  <si>
+    <t>"o"</t>
+  </si>
+  <si>
+    <t>["smpl1", "smpl2", "smpl3", "smpl4"]</t>
+  </si>
+  <si>
+    <t>["smpl1"]</t>
+  </si>
+  <si>
+    <t>"."</t>
+  </si>
+  <si>
+    <t>["smpl3"]</t>
+  </si>
+  <si>
+    <t>["smpl2"]</t>
+  </si>
+  <si>
+    <t>"/"</t>
+  </si>
+  <si>
+    <t>"-"</t>
+  </si>
+  <si>
+    <t>subspecies</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>#00FF00</t>
+  </si>
+  <si>
+    <t>#000077</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>NATIVES</t>
+  </si>
+  <si>
+    <t>$\mathit{Zea\; mays}$ [just-control contaminant]</t>
+  </si>
+  <si>
+    <t>$\mathit{Homo\; sapiens}$ [critical contaminant]</t>
+  </si>
+  <si>
+    <t>$\mathit{Delftia\; acidovorans}$ SPH-1 [native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Delftia\; acidovorans}$ [SPH-1 strain native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Cutibacterium\; acnes}$ [severe contaminant]</t>
+  </si>
+  <si>
+    <t>$\mathit{Salmonella\; enterica}$ subs. enterica [native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Salmonella\; enterica}$ [native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Escherichia\; coli}$ [mild contaminant]</t>
+  </si>
+  <si>
+    <t>$\mathit{Methylobacterium\; radiotolerans}$ [native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Methanosarcina\; mazei}$ [CROSSOVER, smpl1 native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Lactobacillus\; helveticus}$ [native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Methanosarcina\; barkeri}$ [CROSSOVER, smpl3 native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Salmonella\; virus\; Stitch}$ [native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Malassezia\; globosa}$ [other contaminant]</t>
+  </si>
+  <si>
+    <t>$\mathit{Salmonella\; bongori}$ [native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Pan\; troglodytes}$ [mild contaminant]</t>
+  </si>
+  <si>
+    <t>$\mathit{Methanobacterium\; formicicum}$ DSM3637 [native]</t>
+  </si>
+  <si>
+    <t>$\mathit{M.\; formicicum}$ JCM 10132 [other cont.]</t>
+  </si>
+  <si>
+    <t>$\mathit{M.\; formicicum}$ [DSM3637 strain native]</t>
+  </si>
+  <si>
+    <t>$\mathit{Propionibacterium\; virus}$ SKKY [other cont.]</t>
+  </si>
+  <si>
+    <t>$\mathit{Triticum\; aestivum}$ [just-control contaminant]</t>
   </si>
 </sst>
 </file>
@@ -430,7 +593,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -440,8 +603,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -489,16 +654,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -776,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1551,6 +1720,471 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4577</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>9606</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>398578</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>80866</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1747</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>59201</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>28901</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>562</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>31998</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2209</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1587</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2208</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1540099</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>76773</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>54736</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>9598</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1204725</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1300163</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2162</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1982305</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>4565</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="C21" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Use NatMet high-complexity dataset for ROC calculations
On branch master
	modified:   recentrifuge/__init__.py
	modified:   recentrifuge/test/TEST.rcf.html
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
	modified:   retest
	modified:   setup.py
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -1078,25 +1078,25 @@
     <t>HIST</t>
   </si>
   <si>
-    <t>smpl_high</t>
-  </si>
-  <si>
-    <t>["smpl_high"]</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
-    <t>native taxa from NatMet high-complexity dataset for</t>
-  </si>
-  <si>
-    <t>benchmarking metagenomic software (Scyrba et al., 2017)</t>
-  </si>
-  <si>
     <t>Native high-complexity</t>
   </si>
   <si>
     <t>ROOT</t>
+  </si>
+  <si>
+    <t>native taxa from NatMet high-complexity dataset</t>
+  </si>
+  <si>
+    <t>for metagenomics benchmarks (Scyrba et al., 2017)</t>
+  </si>
+  <si>
+    <t>["smplH"]</t>
+  </si>
+  <si>
+    <t>smplH</t>
   </si>
 </sst>
 </file>
@@ -1700,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,7 +1738,7 @@
         <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1770,7 +1770,7 @@
         <v>19496</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1802,7 +1802,7 @@
         <v>10000</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1834,7 +1834,7 @@
         <v>5000</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1866,7 +1866,7 @@
         <v>5000</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1898,7 +1898,7 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1962,7 +1962,7 @@
         <v>5000</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1994,7 +1994,7 @@
         <v>2000</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2026,7 +2026,7 @@
         <v>20</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -2058,7 +2058,7 @@
         <v>15</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2090,7 +2090,7 @@
         <v>5000</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -2136,7 +2136,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E14" s="31">
         <v>1</v>
@@ -2346,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>2995</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -10191,7 +10191,7 @@
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" s="35" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B266">
         <v>1</v>
@@ -10231,7 +10231,7 @@
       </c>
       <c r="D267">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>99996</v>
       </c>
       <c r="E267">
         <f t="shared" si="0"/>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="J267">
         <f t="shared" si="0"/>
-        <v>522878</v>
+        <v>600000</v>
       </c>
     </row>
   </sheetData>
@@ -10269,8 +10269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G263"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:D263"/>
+    <sheetView topLeftCell="A263" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23:E263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10795,13 +10795,13 @@
         <v>107</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D23" t="s">
         <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F23" t="s">
         <v>59</v>
@@ -10818,13 +10818,13 @@
         <v>108</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D24" t="s">
         <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -10841,13 +10841,13 @@
         <v>109</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D25" t="s">
         <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F25" t="s">
         <v>59</v>
@@ -10864,13 +10864,13 @@
         <v>110</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D26" t="s">
         <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -10887,13 +10887,13 @@
         <v>111</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D27" t="s">
         <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>
@@ -10910,13 +10910,13 @@
         <v>112</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D28" t="s">
         <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F28" t="s">
         <v>59</v>
@@ -10933,13 +10933,13 @@
         <v>113</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D29" t="s">
         <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F29" t="s">
         <v>59</v>
@@ -10956,13 +10956,13 @@
         <v>114</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D30" t="s">
         <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F30" t="s">
         <v>59</v>
@@ -10979,13 +10979,13 @@
         <v>115</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D31" t="s">
         <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F31" t="s">
         <v>59</v>
@@ -11002,13 +11002,13 @@
         <v>116</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D32" t="s">
         <v>60</v>
       </c>
       <c r="E32" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F32" t="s">
         <v>59</v>
@@ -11025,13 +11025,13 @@
         <v>117</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D33" t="s">
         <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F33" t="s">
         <v>59</v>
@@ -11048,13 +11048,13 @@
         <v>118</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D34" t="s">
         <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F34" t="s">
         <v>59</v>
@@ -11071,13 +11071,13 @@
         <v>119</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D35" t="s">
         <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F35" t="s">
         <v>59</v>
@@ -11094,13 +11094,13 @@
         <v>120</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D36" t="s">
         <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F36" t="s">
         <v>59</v>
@@ -11117,13 +11117,13 @@
         <v>121</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D37" t="s">
         <v>60</v>
       </c>
       <c r="E37" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F37" t="s">
         <v>59</v>
@@ -11140,13 +11140,13 @@
         <v>122</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D38" t="s">
         <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F38" t="s">
         <v>59</v>
@@ -11163,13 +11163,13 @@
         <v>123</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D39" t="s">
         <v>60</v>
       </c>
       <c r="E39" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F39" t="s">
         <v>59</v>
@@ -11186,13 +11186,13 @@
         <v>124</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D40" t="s">
         <v>60</v>
       </c>
       <c r="E40" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F40" t="s">
         <v>59</v>
@@ -11209,13 +11209,13 @@
         <v>125</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D41" t="s">
         <v>60</v>
       </c>
       <c r="E41" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F41" t="s">
         <v>59</v>
@@ -11232,13 +11232,13 @@
         <v>126</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D42" t="s">
         <v>60</v>
       </c>
       <c r="E42" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F42" t="s">
         <v>59</v>
@@ -11255,13 +11255,13 @@
         <v>127</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D43" t="s">
         <v>60</v>
       </c>
       <c r="E43" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F43" t="s">
         <v>59</v>
@@ -11278,13 +11278,13 @@
         <v>128</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D44" t="s">
         <v>60</v>
       </c>
       <c r="E44" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F44" t="s">
         <v>59</v>
@@ -11301,13 +11301,13 @@
         <v>129</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D45" t="s">
         <v>60</v>
       </c>
       <c r="E45" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F45" t="s">
         <v>59</v>
@@ -11324,13 +11324,13 @@
         <v>130</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D46" t="s">
         <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F46" t="s">
         <v>59</v>
@@ -11347,13 +11347,13 @@
         <v>131</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D47" t="s">
         <v>60</v>
       </c>
       <c r="E47" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F47" t="s">
         <v>59</v>
@@ -11370,13 +11370,13 @@
         <v>132</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D48" t="s">
         <v>60</v>
       </c>
       <c r="E48" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F48" t="s">
         <v>59</v>
@@ -11393,13 +11393,13 @@
         <v>133</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D49" t="s">
         <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F49" t="s">
         <v>59</v>
@@ -11416,13 +11416,13 @@
         <v>134</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D50" t="s">
         <v>60</v>
       </c>
       <c r="E50" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F50" t="s">
         <v>59</v>
@@ -11439,13 +11439,13 @@
         <v>135</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D51" t="s">
         <v>60</v>
       </c>
       <c r="E51" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F51" t="s">
         <v>59</v>
@@ -11462,13 +11462,13 @@
         <v>136</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D52" t="s">
         <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F52" t="s">
         <v>59</v>
@@ -11485,13 +11485,13 @@
         <v>137</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D53" t="s">
         <v>60</v>
       </c>
       <c r="E53" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F53" t="s">
         <v>59</v>
@@ -11508,13 +11508,13 @@
         <v>138</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D54" t="s">
         <v>60</v>
       </c>
       <c r="E54" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F54" t="s">
         <v>59</v>
@@ -11531,13 +11531,13 @@
         <v>139</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D55" t="s">
         <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F55" t="s">
         <v>59</v>
@@ -11554,13 +11554,13 @@
         <v>140</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D56" t="s">
         <v>60</v>
       </c>
       <c r="E56" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F56" t="s">
         <v>59</v>
@@ -11577,13 +11577,13 @@
         <v>141</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D57" t="s">
         <v>60</v>
       </c>
       <c r="E57" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F57" t="s">
         <v>59</v>
@@ -11600,13 +11600,13 @@
         <v>142</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
       </c>
       <c r="E58" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F58" t="s">
         <v>59</v>
@@ -11623,13 +11623,13 @@
         <v>143</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D59" t="s">
         <v>60</v>
       </c>
       <c r="E59" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F59" t="s">
         <v>59</v>
@@ -11646,13 +11646,13 @@
         <v>144</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D60" t="s">
         <v>60</v>
       </c>
       <c r="E60" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F60" t="s">
         <v>59</v>
@@ -11669,13 +11669,13 @@
         <v>145</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D61" t="s">
         <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F61" t="s">
         <v>59</v>
@@ -11692,13 +11692,13 @@
         <v>146</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D62" t="s">
         <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F62" t="s">
         <v>59</v>
@@ -11715,13 +11715,13 @@
         <v>147</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D63" t="s">
         <v>60</v>
       </c>
       <c r="E63" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F63" t="s">
         <v>59</v>
@@ -11738,13 +11738,13 @@
         <v>148</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D64" t="s">
         <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F64" t="s">
         <v>59</v>
@@ -11761,13 +11761,13 @@
         <v>149</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D65" t="s">
         <v>60</v>
       </c>
       <c r="E65" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F65" t="s">
         <v>59</v>
@@ -11784,13 +11784,13 @@
         <v>150</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D66" t="s">
         <v>60</v>
       </c>
       <c r="E66" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F66" t="s">
         <v>59</v>
@@ -11807,13 +11807,13 @@
         <v>151</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D67" t="s">
         <v>60</v>
       </c>
       <c r="E67" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F67" t="s">
         <v>59</v>
@@ -11830,13 +11830,13 @@
         <v>152</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D68" t="s">
         <v>60</v>
       </c>
       <c r="E68" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F68" t="s">
         <v>59</v>
@@ -11853,13 +11853,13 @@
         <v>153</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D69" t="s">
         <v>60</v>
       </c>
       <c r="E69" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F69" t="s">
         <v>59</v>
@@ -11876,13 +11876,13 @@
         <v>154</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D70" t="s">
         <v>60</v>
       </c>
       <c r="E70" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F70" t="s">
         <v>59</v>
@@ -11899,13 +11899,13 @@
         <v>155</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D71" t="s">
         <v>60</v>
       </c>
       <c r="E71" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F71" t="s">
         <v>59</v>
@@ -11922,13 +11922,13 @@
         <v>156</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D72" t="s">
         <v>60</v>
       </c>
       <c r="E72" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F72" t="s">
         <v>59</v>
@@ -11945,13 +11945,13 @@
         <v>157</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D73" t="s">
         <v>60</v>
       </c>
       <c r="E73" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F73" t="s">
         <v>59</v>
@@ -11968,13 +11968,13 @@
         <v>158</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D74" t="s">
         <v>60</v>
       </c>
       <c r="E74" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F74" t="s">
         <v>59</v>
@@ -11991,13 +11991,13 @@
         <v>159</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D75" t="s">
         <v>60</v>
       </c>
       <c r="E75" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F75" t="s">
         <v>59</v>
@@ -12014,13 +12014,13 @@
         <v>160</v>
       </c>
       <c r="C76" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D76" t="s">
         <v>60</v>
       </c>
       <c r="E76" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F76" t="s">
         <v>59</v>
@@ -12037,13 +12037,13 @@
         <v>161</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D77" t="s">
         <v>60</v>
       </c>
       <c r="E77" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F77" t="s">
         <v>59</v>
@@ -12060,13 +12060,13 @@
         <v>162</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D78" t="s">
         <v>60</v>
       </c>
       <c r="E78" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F78" t="s">
         <v>59</v>
@@ -12083,13 +12083,13 @@
         <v>163</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D79" t="s">
         <v>60</v>
       </c>
       <c r="E79" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F79" t="s">
         <v>59</v>
@@ -12106,13 +12106,13 @@
         <v>164</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D80" t="s">
         <v>60</v>
       </c>
       <c r="E80" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F80" t="s">
         <v>59</v>
@@ -12129,13 +12129,13 @@
         <v>165</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D81" t="s">
         <v>60</v>
       </c>
       <c r="E81" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F81" t="s">
         <v>59</v>
@@ -12152,13 +12152,13 @@
         <v>166</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D82" t="s">
         <v>60</v>
       </c>
       <c r="E82" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F82" t="s">
         <v>59</v>
@@ -12175,13 +12175,13 @@
         <v>167</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D83" t="s">
         <v>60</v>
       </c>
       <c r="E83" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F83" t="s">
         <v>59</v>
@@ -12198,13 +12198,13 @@
         <v>168</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D84" t="s">
         <v>60</v>
       </c>
       <c r="E84" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F84" t="s">
         <v>59</v>
@@ -12221,13 +12221,13 @@
         <v>169</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D85" t="s">
         <v>60</v>
       </c>
       <c r="E85" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F85" t="s">
         <v>59</v>
@@ -12244,13 +12244,13 @@
         <v>170</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D86" t="s">
         <v>60</v>
       </c>
       <c r="E86" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F86" t="s">
         <v>59</v>
@@ -12267,13 +12267,13 @@
         <v>171</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D87" t="s">
         <v>60</v>
       </c>
       <c r="E87" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F87" t="s">
         <v>59</v>
@@ -12290,13 +12290,13 @@
         <v>172</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D88" t="s">
         <v>60</v>
       </c>
       <c r="E88" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F88" t="s">
         <v>59</v>
@@ -12313,13 +12313,13 @@
         <v>173</v>
       </c>
       <c r="C89" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D89" t="s">
         <v>60</v>
       </c>
       <c r="E89" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F89" t="s">
         <v>59</v>
@@ -12336,13 +12336,13 @@
         <v>174</v>
       </c>
       <c r="C90" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D90" t="s">
         <v>60</v>
       </c>
       <c r="E90" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F90" t="s">
         <v>59</v>
@@ -12359,13 +12359,13 @@
         <v>175</v>
       </c>
       <c r="C91" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D91" t="s">
         <v>60</v>
       </c>
       <c r="E91" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F91" t="s">
         <v>59</v>
@@ -12382,13 +12382,13 @@
         <v>176</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D92" t="s">
         <v>60</v>
       </c>
       <c r="E92" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F92" t="s">
         <v>59</v>
@@ -12405,13 +12405,13 @@
         <v>177</v>
       </c>
       <c r="C93" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D93" t="s">
         <v>60</v>
       </c>
       <c r="E93" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F93" t="s">
         <v>59</v>
@@ -12428,13 +12428,13 @@
         <v>178</v>
       </c>
       <c r="C94" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D94" t="s">
         <v>60</v>
       </c>
       <c r="E94" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F94" t="s">
         <v>59</v>
@@ -12451,13 +12451,13 @@
         <v>179</v>
       </c>
       <c r="C95" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D95" t="s">
         <v>60</v>
       </c>
       <c r="E95" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F95" t="s">
         <v>59</v>
@@ -12474,13 +12474,13 @@
         <v>180</v>
       </c>
       <c r="C96" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D96" t="s">
         <v>60</v>
       </c>
       <c r="E96" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F96" t="s">
         <v>59</v>
@@ -12497,13 +12497,13 @@
         <v>181</v>
       </c>
       <c r="C97" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D97" t="s">
         <v>60</v>
       </c>
       <c r="E97" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F97" t="s">
         <v>59</v>
@@ -12520,13 +12520,13 @@
         <v>182</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D98" t="s">
         <v>60</v>
       </c>
       <c r="E98" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F98" t="s">
         <v>59</v>
@@ -12543,13 +12543,13 @@
         <v>183</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D99" t="s">
         <v>60</v>
       </c>
       <c r="E99" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F99" t="s">
         <v>59</v>
@@ -12566,13 +12566,13 @@
         <v>184</v>
       </c>
       <c r="C100" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D100" t="s">
         <v>60</v>
       </c>
       <c r="E100" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F100" t="s">
         <v>59</v>
@@ -12589,13 +12589,13 @@
         <v>185</v>
       </c>
       <c r="C101" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D101" t="s">
         <v>60</v>
       </c>
       <c r="E101" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F101" t="s">
         <v>59</v>
@@ -12612,13 +12612,13 @@
         <v>186</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D102" t="s">
         <v>60</v>
       </c>
       <c r="E102" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F102" t="s">
         <v>59</v>
@@ -12635,13 +12635,13 @@
         <v>187</v>
       </c>
       <c r="C103" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D103" t="s">
         <v>60</v>
       </c>
       <c r="E103" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F103" t="s">
         <v>59</v>
@@ -12658,13 +12658,13 @@
         <v>188</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D104" t="s">
         <v>60</v>
       </c>
       <c r="E104" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F104" t="s">
         <v>59</v>
@@ -12681,13 +12681,13 @@
         <v>189</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D105" t="s">
         <v>60</v>
       </c>
       <c r="E105" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F105" t="s">
         <v>59</v>
@@ -12704,13 +12704,13 @@
         <v>190</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D106" t="s">
         <v>60</v>
       </c>
       <c r="E106" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F106" t="s">
         <v>59</v>
@@ -12727,13 +12727,13 @@
         <v>191</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D107" t="s">
         <v>60</v>
       </c>
       <c r="E107" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F107" t="s">
         <v>59</v>
@@ -12750,13 +12750,13 @@
         <v>192</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D108" t="s">
         <v>60</v>
       </c>
       <c r="E108" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F108" t="s">
         <v>59</v>
@@ -12773,13 +12773,13 @@
         <v>193</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D109" t="s">
         <v>60</v>
       </c>
       <c r="E109" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F109" t="s">
         <v>59</v>
@@ -12796,13 +12796,13 @@
         <v>194</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D110" t="s">
         <v>60</v>
       </c>
       <c r="E110" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F110" t="s">
         <v>59</v>
@@ -12819,13 +12819,13 @@
         <v>195</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D111" t="s">
         <v>60</v>
       </c>
       <c r="E111" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F111" t="s">
         <v>59</v>
@@ -12842,13 +12842,13 @@
         <v>196</v>
       </c>
       <c r="C112" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D112" t="s">
         <v>60</v>
       </c>
       <c r="E112" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F112" t="s">
         <v>59</v>
@@ -12865,13 +12865,13 @@
         <v>197</v>
       </c>
       <c r="C113" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D113" t="s">
         <v>60</v>
       </c>
       <c r="E113" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F113" t="s">
         <v>59</v>
@@ -12888,13 +12888,13 @@
         <v>198</v>
       </c>
       <c r="C114" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D114" t="s">
         <v>60</v>
       </c>
       <c r="E114" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F114" t="s">
         <v>59</v>
@@ -12911,13 +12911,13 @@
         <v>199</v>
       </c>
       <c r="C115" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D115" t="s">
         <v>60</v>
       </c>
       <c r="E115" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F115" t="s">
         <v>59</v>
@@ -12934,13 +12934,13 @@
         <v>200</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D116" t="s">
         <v>60</v>
       </c>
       <c r="E116" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F116" t="s">
         <v>59</v>
@@ -12957,13 +12957,13 @@
         <v>201</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D117" t="s">
         <v>60</v>
       </c>
       <c r="E117" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F117" t="s">
         <v>59</v>
@@ -12980,13 +12980,13 @@
         <v>202</v>
       </c>
       <c r="C118" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D118" t="s">
         <v>60</v>
       </c>
       <c r="E118" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F118" t="s">
         <v>59</v>
@@ -13003,13 +13003,13 @@
         <v>203</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D119" t="s">
         <v>60</v>
       </c>
       <c r="E119" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F119" t="s">
         <v>59</v>
@@ -13026,13 +13026,13 @@
         <v>204</v>
       </c>
       <c r="C120" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D120" t="s">
         <v>60</v>
       </c>
       <c r="E120" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F120" t="s">
         <v>59</v>
@@ -13049,13 +13049,13 @@
         <v>205</v>
       </c>
       <c r="C121" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D121" t="s">
         <v>60</v>
       </c>
       <c r="E121" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F121" t="s">
         <v>59</v>
@@ -13072,13 +13072,13 @@
         <v>206</v>
       </c>
       <c r="C122" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D122" t="s">
         <v>60</v>
       </c>
       <c r="E122" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F122" t="s">
         <v>59</v>
@@ -13095,13 +13095,13 @@
         <v>207</v>
       </c>
       <c r="C123" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D123" t="s">
         <v>60</v>
       </c>
       <c r="E123" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F123" t="s">
         <v>59</v>
@@ -13118,13 +13118,13 @@
         <v>208</v>
       </c>
       <c r="C124" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D124" t="s">
         <v>60</v>
       </c>
       <c r="E124" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F124" t="s">
         <v>59</v>
@@ -13141,13 +13141,13 @@
         <v>209</v>
       </c>
       <c r="C125" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D125" t="s">
         <v>60</v>
       </c>
       <c r="E125" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F125" t="s">
         <v>59</v>
@@ -13164,13 +13164,13 @@
         <v>210</v>
       </c>
       <c r="C126" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D126" t="s">
         <v>60</v>
       </c>
       <c r="E126" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F126" t="s">
         <v>59</v>
@@ -13187,13 +13187,13 @@
         <v>211</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D127" t="s">
         <v>60</v>
       </c>
       <c r="E127" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F127" t="s">
         <v>59</v>
@@ -13210,13 +13210,13 @@
         <v>212</v>
       </c>
       <c r="C128" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D128" t="s">
         <v>60</v>
       </c>
       <c r="E128" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F128" t="s">
         <v>59</v>
@@ -13233,13 +13233,13 @@
         <v>213</v>
       </c>
       <c r="C129" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D129" t="s">
         <v>60</v>
       </c>
       <c r="E129" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F129" t="s">
         <v>59</v>
@@ -13256,13 +13256,13 @@
         <v>214</v>
       </c>
       <c r="C130" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D130" t="s">
         <v>60</v>
       </c>
       <c r="E130" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F130" t="s">
         <v>59</v>
@@ -13279,13 +13279,13 @@
         <v>215</v>
       </c>
       <c r="C131" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D131" t="s">
         <v>60</v>
       </c>
       <c r="E131" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F131" t="s">
         <v>59</v>
@@ -13302,13 +13302,13 @@
         <v>216</v>
       </c>
       <c r="C132" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D132" t="s">
         <v>60</v>
       </c>
       <c r="E132" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F132" t="s">
         <v>59</v>
@@ -13325,13 +13325,13 @@
         <v>217</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D133" t="s">
         <v>60</v>
       </c>
       <c r="E133" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F133" t="s">
         <v>59</v>
@@ -13348,13 +13348,13 @@
         <v>218</v>
       </c>
       <c r="C134" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D134" t="s">
         <v>60</v>
       </c>
       <c r="E134" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F134" t="s">
         <v>59</v>
@@ -13371,13 +13371,13 @@
         <v>219</v>
       </c>
       <c r="C135" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D135" t="s">
         <v>60</v>
       </c>
       <c r="E135" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F135" t="s">
         <v>59</v>
@@ -13394,13 +13394,13 @@
         <v>220</v>
       </c>
       <c r="C136" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D136" t="s">
         <v>60</v>
       </c>
       <c r="E136" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F136" t="s">
         <v>59</v>
@@ -13417,13 +13417,13 @@
         <v>221</v>
       </c>
       <c r="C137" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D137" t="s">
         <v>60</v>
       </c>
       <c r="E137" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F137" t="s">
         <v>59</v>
@@ -13440,13 +13440,13 @@
         <v>222</v>
       </c>
       <c r="C138" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D138" t="s">
         <v>60</v>
       </c>
       <c r="E138" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F138" t="s">
         <v>59</v>
@@ -13463,13 +13463,13 @@
         <v>223</v>
       </c>
       <c r="C139" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D139" t="s">
         <v>60</v>
       </c>
       <c r="E139" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F139" t="s">
         <v>59</v>
@@ -13486,13 +13486,13 @@
         <v>224</v>
       </c>
       <c r="C140" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D140" t="s">
         <v>60</v>
       </c>
       <c r="E140" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F140" t="s">
         <v>59</v>
@@ -13509,13 +13509,13 @@
         <v>225</v>
       </c>
       <c r="C141" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D141" t="s">
         <v>60</v>
       </c>
       <c r="E141" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F141" t="s">
         <v>59</v>
@@ -13532,13 +13532,13 @@
         <v>226</v>
       </c>
       <c r="C142" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D142" t="s">
         <v>60</v>
       </c>
       <c r="E142" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F142" t="s">
         <v>59</v>
@@ -13555,13 +13555,13 @@
         <v>227</v>
       </c>
       <c r="C143" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D143" t="s">
         <v>60</v>
       </c>
       <c r="E143" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F143" t="s">
         <v>59</v>
@@ -13578,13 +13578,13 @@
         <v>228</v>
       </c>
       <c r="C144" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D144" t="s">
         <v>60</v>
       </c>
       <c r="E144" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F144" t="s">
         <v>59</v>
@@ -13601,13 +13601,13 @@
         <v>229</v>
       </c>
       <c r="C145" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D145" t="s">
         <v>60</v>
       </c>
       <c r="E145" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F145" t="s">
         <v>59</v>
@@ -13624,13 +13624,13 @@
         <v>230</v>
       </c>
       <c r="C146" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D146" t="s">
         <v>60</v>
       </c>
       <c r="E146" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F146" t="s">
         <v>59</v>
@@ -13647,13 +13647,13 @@
         <v>231</v>
       </c>
       <c r="C147" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D147" t="s">
         <v>60</v>
       </c>
       <c r="E147" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F147" t="s">
         <v>59</v>
@@ -13670,13 +13670,13 @@
         <v>232</v>
       </c>
       <c r="C148" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D148" t="s">
         <v>60</v>
       </c>
       <c r="E148" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F148" t="s">
         <v>59</v>
@@ -13693,13 +13693,13 @@
         <v>233</v>
       </c>
       <c r="C149" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D149" t="s">
         <v>60</v>
       </c>
       <c r="E149" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F149" t="s">
         <v>59</v>
@@ -13716,13 +13716,13 @@
         <v>234</v>
       </c>
       <c r="C150" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D150" t="s">
         <v>60</v>
       </c>
       <c r="E150" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F150" t="s">
         <v>59</v>
@@ -13739,13 +13739,13 @@
         <v>235</v>
       </c>
       <c r="C151" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D151" t="s">
         <v>60</v>
       </c>
       <c r="E151" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F151" t="s">
         <v>59</v>
@@ -13762,13 +13762,13 @@
         <v>236</v>
       </c>
       <c r="C152" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D152" t="s">
         <v>60</v>
       </c>
       <c r="E152" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F152" t="s">
         <v>59</v>
@@ -13785,13 +13785,13 @@
         <v>237</v>
       </c>
       <c r="C153" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D153" t="s">
         <v>60</v>
       </c>
       <c r="E153" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F153" t="s">
         <v>59</v>
@@ -13808,13 +13808,13 @@
         <v>238</v>
       </c>
       <c r="C154" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D154" t="s">
         <v>60</v>
       </c>
       <c r="E154" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F154" t="s">
         <v>59</v>
@@ -13831,13 +13831,13 @@
         <v>239</v>
       </c>
       <c r="C155" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D155" t="s">
         <v>60</v>
       </c>
       <c r="E155" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F155" t="s">
         <v>59</v>
@@ -13854,13 +13854,13 @@
         <v>240</v>
       </c>
       <c r="C156" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D156" t="s">
         <v>60</v>
       </c>
       <c r="E156" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F156" t="s">
         <v>59</v>
@@ -13877,13 +13877,13 @@
         <v>241</v>
       </c>
       <c r="C157" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D157" t="s">
         <v>60</v>
       </c>
       <c r="E157" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F157" t="s">
         <v>59</v>
@@ -13900,13 +13900,13 @@
         <v>242</v>
       </c>
       <c r="C158" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D158" t="s">
         <v>60</v>
       </c>
       <c r="E158" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F158" t="s">
         <v>59</v>
@@ -13923,13 +13923,13 @@
         <v>243</v>
       </c>
       <c r="C159" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D159" t="s">
         <v>60</v>
       </c>
       <c r="E159" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F159" t="s">
         <v>59</v>
@@ -13946,13 +13946,13 @@
         <v>244</v>
       </c>
       <c r="C160" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D160" t="s">
         <v>60</v>
       </c>
       <c r="E160" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F160" t="s">
         <v>59</v>
@@ -13969,13 +13969,13 @@
         <v>245</v>
       </c>
       <c r="C161" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D161" t="s">
         <v>60</v>
       </c>
       <c r="E161" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F161" t="s">
         <v>59</v>
@@ -13992,13 +13992,13 @@
         <v>246</v>
       </c>
       <c r="C162" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D162" t="s">
         <v>60</v>
       </c>
       <c r="E162" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F162" t="s">
         <v>59</v>
@@ -14015,13 +14015,13 @@
         <v>247</v>
       </c>
       <c r="C163" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D163" t="s">
         <v>60</v>
       </c>
       <c r="E163" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F163" t="s">
         <v>59</v>
@@ -14038,13 +14038,13 @@
         <v>248</v>
       </c>
       <c r="C164" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D164" t="s">
         <v>60</v>
       </c>
       <c r="E164" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F164" t="s">
         <v>59</v>
@@ -14061,13 +14061,13 @@
         <v>249</v>
       </c>
       <c r="C165" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D165" t="s">
         <v>60</v>
       </c>
       <c r="E165" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F165" t="s">
         <v>59</v>
@@ -14084,13 +14084,13 @@
         <v>250</v>
       </c>
       <c r="C166" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D166" t="s">
         <v>60</v>
       </c>
       <c r="E166" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F166" t="s">
         <v>59</v>
@@ -14107,13 +14107,13 @@
         <v>251</v>
       </c>
       <c r="C167" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D167" t="s">
         <v>60</v>
       </c>
       <c r="E167" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F167" t="s">
         <v>59</v>
@@ -14130,13 +14130,13 @@
         <v>252</v>
       </c>
       <c r="C168" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D168" t="s">
         <v>60</v>
       </c>
       <c r="E168" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F168" t="s">
         <v>59</v>
@@ -14153,13 +14153,13 @@
         <v>253</v>
       </c>
       <c r="C169" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D169" t="s">
         <v>60</v>
       </c>
       <c r="E169" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F169" t="s">
         <v>59</v>
@@ -14176,13 +14176,13 @@
         <v>254</v>
       </c>
       <c r="C170" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D170" t="s">
         <v>60</v>
       </c>
       <c r="E170" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F170" t="s">
         <v>59</v>
@@ -14199,13 +14199,13 @@
         <v>255</v>
       </c>
       <c r="C171" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D171" t="s">
         <v>60</v>
       </c>
       <c r="E171" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F171" t="s">
         <v>59</v>
@@ -14222,13 +14222,13 @@
         <v>256</v>
       </c>
       <c r="C172" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D172" t="s">
         <v>60</v>
       </c>
       <c r="E172" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F172" t="s">
         <v>59</v>
@@ -14245,13 +14245,13 @@
         <v>257</v>
       </c>
       <c r="C173" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D173" t="s">
         <v>60</v>
       </c>
       <c r="E173" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F173" t="s">
         <v>59</v>
@@ -14268,13 +14268,13 @@
         <v>258</v>
       </c>
       <c r="C174" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D174" t="s">
         <v>60</v>
       </c>
       <c r="E174" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F174" t="s">
         <v>59</v>
@@ -14291,13 +14291,13 @@
         <v>259</v>
       </c>
       <c r="C175" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D175" t="s">
         <v>60</v>
       </c>
       <c r="E175" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F175" t="s">
         <v>59</v>
@@ -14314,13 +14314,13 @@
         <v>260</v>
       </c>
       <c r="C176" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D176" t="s">
         <v>60</v>
       </c>
       <c r="E176" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F176" t="s">
         <v>59</v>
@@ -14337,13 +14337,13 @@
         <v>261</v>
       </c>
       <c r="C177" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D177" t="s">
         <v>60</v>
       </c>
       <c r="E177" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F177" t="s">
         <v>59</v>
@@ -14360,13 +14360,13 @@
         <v>262</v>
       </c>
       <c r="C178" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D178" t="s">
         <v>60</v>
       </c>
       <c r="E178" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F178" t="s">
         <v>59</v>
@@ -14383,13 +14383,13 @@
         <v>263</v>
       </c>
       <c r="C179" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D179" t="s">
         <v>60</v>
       </c>
       <c r="E179" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F179" t="s">
         <v>59</v>
@@ -14406,13 +14406,13 @@
         <v>264</v>
       </c>
       <c r="C180" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D180" t="s">
         <v>60</v>
       </c>
       <c r="E180" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F180" t="s">
         <v>59</v>
@@ -14429,13 +14429,13 @@
         <v>265</v>
       </c>
       <c r="C181" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D181" t="s">
         <v>60</v>
       </c>
       <c r="E181" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F181" t="s">
         <v>59</v>
@@ -14452,13 +14452,13 @@
         <v>266</v>
       </c>
       <c r="C182" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D182" t="s">
         <v>60</v>
       </c>
       <c r="E182" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F182" t="s">
         <v>59</v>
@@ -14475,13 +14475,13 @@
         <v>267</v>
       </c>
       <c r="C183" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D183" t="s">
         <v>60</v>
       </c>
       <c r="E183" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F183" t="s">
         <v>59</v>
@@ -14498,13 +14498,13 @@
         <v>268</v>
       </c>
       <c r="C184" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D184" t="s">
         <v>60</v>
       </c>
       <c r="E184" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F184" t="s">
         <v>59</v>
@@ -14521,13 +14521,13 @@
         <v>269</v>
       </c>
       <c r="C185" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D185" t="s">
         <v>60</v>
       </c>
       <c r="E185" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F185" t="s">
         <v>59</v>
@@ -14544,13 +14544,13 @@
         <v>270</v>
       </c>
       <c r="C186" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D186" t="s">
         <v>60</v>
       </c>
       <c r="E186" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F186" t="s">
         <v>59</v>
@@ -14567,13 +14567,13 @@
         <v>271</v>
       </c>
       <c r="C187" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D187" t="s">
         <v>60</v>
       </c>
       <c r="E187" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F187" t="s">
         <v>59</v>
@@ -14590,13 +14590,13 @@
         <v>272</v>
       </c>
       <c r="C188" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D188" t="s">
         <v>60</v>
       </c>
       <c r="E188" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F188" t="s">
         <v>59</v>
@@ -14613,13 +14613,13 @@
         <v>273</v>
       </c>
       <c r="C189" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D189" t="s">
         <v>60</v>
       </c>
       <c r="E189" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F189" t="s">
         <v>59</v>
@@ -14636,13 +14636,13 @@
         <v>274</v>
       </c>
       <c r="C190" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D190" t="s">
         <v>60</v>
       </c>
       <c r="E190" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F190" t="s">
         <v>59</v>
@@ -14659,13 +14659,13 @@
         <v>275</v>
       </c>
       <c r="C191" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D191" t="s">
         <v>60</v>
       </c>
       <c r="E191" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F191" t="s">
         <v>59</v>
@@ -14682,13 +14682,13 @@
         <v>276</v>
       </c>
       <c r="C192" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D192" t="s">
         <v>60</v>
       </c>
       <c r="E192" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F192" t="s">
         <v>59</v>
@@ -14705,13 +14705,13 @@
         <v>277</v>
       </c>
       <c r="C193" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D193" t="s">
         <v>60</v>
       </c>
       <c r="E193" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F193" t="s">
         <v>59</v>
@@ -14728,13 +14728,13 @@
         <v>278</v>
       </c>
       <c r="C194" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D194" t="s">
         <v>60</v>
       </c>
       <c r="E194" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F194" t="s">
         <v>59</v>
@@ -14751,13 +14751,13 @@
         <v>279</v>
       </c>
       <c r="C195" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D195" t="s">
         <v>60</v>
       </c>
       <c r="E195" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F195" t="s">
         <v>59</v>
@@ -14774,13 +14774,13 @@
         <v>280</v>
       </c>
       <c r="C196" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D196" t="s">
         <v>60</v>
       </c>
       <c r="E196" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F196" t="s">
         <v>59</v>
@@ -14797,13 +14797,13 @@
         <v>281</v>
       </c>
       <c r="C197" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D197" t="s">
         <v>60</v>
       </c>
       <c r="E197" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F197" t="s">
         <v>59</v>
@@ -14820,13 +14820,13 @@
         <v>282</v>
       </c>
       <c r="C198" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D198" t="s">
         <v>60</v>
       </c>
       <c r="E198" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F198" t="s">
         <v>59</v>
@@ -14843,13 +14843,13 @@
         <v>283</v>
       </c>
       <c r="C199" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D199" t="s">
         <v>60</v>
       </c>
       <c r="E199" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F199" t="s">
         <v>59</v>
@@ -14866,13 +14866,13 @@
         <v>284</v>
       </c>
       <c r="C200" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D200" t="s">
         <v>60</v>
       </c>
       <c r="E200" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F200" t="s">
         <v>59</v>
@@ -14889,13 +14889,13 @@
         <v>285</v>
       </c>
       <c r="C201" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D201" t="s">
         <v>60</v>
       </c>
       <c r="E201" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F201" t="s">
         <v>59</v>
@@ -14912,13 +14912,13 @@
         <v>286</v>
       </c>
       <c r="C202" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D202" t="s">
         <v>60</v>
       </c>
       <c r="E202" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F202" t="s">
         <v>59</v>
@@ -14935,13 +14935,13 @@
         <v>287</v>
       </c>
       <c r="C203" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D203" t="s">
         <v>60</v>
       </c>
       <c r="E203" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F203" t="s">
         <v>59</v>
@@ -14958,13 +14958,13 @@
         <v>288</v>
       </c>
       <c r="C204" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D204" t="s">
         <v>60</v>
       </c>
       <c r="E204" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F204" t="s">
         <v>59</v>
@@ -14981,13 +14981,13 @@
         <v>289</v>
       </c>
       <c r="C205" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D205" t="s">
         <v>60</v>
       </c>
       <c r="E205" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F205" t="s">
         <v>59</v>
@@ -15004,13 +15004,13 @@
         <v>290</v>
       </c>
       <c r="C206" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D206" t="s">
         <v>60</v>
       </c>
       <c r="E206" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F206" t="s">
         <v>59</v>
@@ -15027,13 +15027,13 @@
         <v>291</v>
       </c>
       <c r="C207" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D207" t="s">
         <v>60</v>
       </c>
       <c r="E207" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F207" t="s">
         <v>59</v>
@@ -15050,13 +15050,13 @@
         <v>292</v>
       </c>
       <c r="C208" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D208" t="s">
         <v>60</v>
       </c>
       <c r="E208" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F208" t="s">
         <v>59</v>
@@ -15073,13 +15073,13 @@
         <v>293</v>
       </c>
       <c r="C209" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D209" t="s">
         <v>60</v>
       </c>
       <c r="E209" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F209" t="s">
         <v>59</v>
@@ -15096,13 +15096,13 @@
         <v>294</v>
       </c>
       <c r="C210" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D210" t="s">
         <v>60</v>
       </c>
       <c r="E210" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F210" t="s">
         <v>59</v>
@@ -15119,13 +15119,13 @@
         <v>295</v>
       </c>
       <c r="C211" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D211" t="s">
         <v>60</v>
       </c>
       <c r="E211" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F211" t="s">
         <v>59</v>
@@ -15142,13 +15142,13 @@
         <v>296</v>
       </c>
       <c r="C212" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D212" t="s">
         <v>60</v>
       </c>
       <c r="E212" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F212" t="s">
         <v>59</v>
@@ -15165,13 +15165,13 @@
         <v>297</v>
       </c>
       <c r="C213" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D213" t="s">
         <v>60</v>
       </c>
       <c r="E213" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F213" t="s">
         <v>59</v>
@@ -15188,13 +15188,13 @@
         <v>298</v>
       </c>
       <c r="C214" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D214" t="s">
         <v>60</v>
       </c>
       <c r="E214" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F214" t="s">
         <v>59</v>
@@ -15211,13 +15211,13 @@
         <v>299</v>
       </c>
       <c r="C215" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D215" t="s">
         <v>60</v>
       </c>
       <c r="E215" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F215" t="s">
         <v>59</v>
@@ -15234,13 +15234,13 @@
         <v>300</v>
       </c>
       <c r="C216" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D216" t="s">
         <v>60</v>
       </c>
       <c r="E216" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F216" t="s">
         <v>59</v>
@@ -15257,13 +15257,13 @@
         <v>301</v>
       </c>
       <c r="C217" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D217" t="s">
         <v>60</v>
       </c>
       <c r="E217" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F217" t="s">
         <v>59</v>
@@ -15280,13 +15280,13 @@
         <v>302</v>
       </c>
       <c r="C218" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D218" t="s">
         <v>60</v>
       </c>
       <c r="E218" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F218" t="s">
         <v>59</v>
@@ -15303,13 +15303,13 @@
         <v>303</v>
       </c>
       <c r="C219" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D219" t="s">
         <v>60</v>
       </c>
       <c r="E219" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F219" t="s">
         <v>59</v>
@@ -15326,13 +15326,13 @@
         <v>304</v>
       </c>
       <c r="C220" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D220" t="s">
         <v>60</v>
       </c>
       <c r="E220" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F220" t="s">
         <v>59</v>
@@ -15349,13 +15349,13 @@
         <v>305</v>
       </c>
       <c r="C221" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D221" t="s">
         <v>60</v>
       </c>
       <c r="E221" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F221" t="s">
         <v>59</v>
@@ -15372,13 +15372,13 @@
         <v>306</v>
       </c>
       <c r="C222" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D222" t="s">
         <v>60</v>
       </c>
       <c r="E222" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F222" t="s">
         <v>59</v>
@@ -15395,13 +15395,13 @@
         <v>307</v>
       </c>
       <c r="C223" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D223" t="s">
         <v>60</v>
       </c>
       <c r="E223" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F223" t="s">
         <v>59</v>
@@ -15418,13 +15418,13 @@
         <v>308</v>
       </c>
       <c r="C224" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D224" t="s">
         <v>60</v>
       </c>
       <c r="E224" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F224" t="s">
         <v>59</v>
@@ -15441,13 +15441,13 @@
         <v>309</v>
       </c>
       <c r="C225" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D225" t="s">
         <v>60</v>
       </c>
       <c r="E225" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F225" t="s">
         <v>59</v>
@@ -15464,13 +15464,13 @@
         <v>310</v>
       </c>
       <c r="C226" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D226" t="s">
         <v>60</v>
       </c>
       <c r="E226" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F226" t="s">
         <v>59</v>
@@ -15487,13 +15487,13 @@
         <v>311</v>
       </c>
       <c r="C227" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D227" t="s">
         <v>60</v>
       </c>
       <c r="E227" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F227" t="s">
         <v>59</v>
@@ -15510,13 +15510,13 @@
         <v>312</v>
       </c>
       <c r="C228" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D228" t="s">
         <v>60</v>
       </c>
       <c r="E228" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F228" t="s">
         <v>59</v>
@@ -15533,13 +15533,13 @@
         <v>313</v>
       </c>
       <c r="C229" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D229" t="s">
         <v>60</v>
       </c>
       <c r="E229" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F229" t="s">
         <v>59</v>
@@ -15556,13 +15556,13 @@
         <v>314</v>
       </c>
       <c r="C230" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D230" t="s">
         <v>60</v>
       </c>
       <c r="E230" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F230" t="s">
         <v>59</v>
@@ -15579,13 +15579,13 @@
         <v>315</v>
       </c>
       <c r="C231" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D231" t="s">
         <v>60</v>
       </c>
       <c r="E231" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F231" t="s">
         <v>59</v>
@@ -15602,13 +15602,13 @@
         <v>316</v>
       </c>
       <c r="C232" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D232" t="s">
         <v>60</v>
       </c>
       <c r="E232" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F232" t="s">
         <v>59</v>
@@ -15625,13 +15625,13 @@
         <v>317</v>
       </c>
       <c r="C233" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D233" t="s">
         <v>60</v>
       </c>
       <c r="E233" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F233" t="s">
         <v>59</v>
@@ -15648,13 +15648,13 @@
         <v>318</v>
       </c>
       <c r="C234" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D234" t="s">
         <v>60</v>
       </c>
       <c r="E234" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F234" t="s">
         <v>59</v>
@@ -15671,13 +15671,13 @@
         <v>319</v>
       </c>
       <c r="C235" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D235" t="s">
         <v>60</v>
       </c>
       <c r="E235" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F235" t="s">
         <v>59</v>
@@ -15694,13 +15694,13 @@
         <v>320</v>
       </c>
       <c r="C236" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D236" t="s">
         <v>60</v>
       </c>
       <c r="E236" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F236" t="s">
         <v>59</v>
@@ -15717,13 +15717,13 @@
         <v>321</v>
       </c>
       <c r="C237" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D237" t="s">
         <v>60</v>
       </c>
       <c r="E237" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F237" t="s">
         <v>59</v>
@@ -15740,13 +15740,13 @@
         <v>322</v>
       </c>
       <c r="C238" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D238" t="s">
         <v>60</v>
       </c>
       <c r="E238" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F238" t="s">
         <v>59</v>
@@ -15763,13 +15763,13 @@
         <v>323</v>
       </c>
       <c r="C239" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D239" t="s">
         <v>60</v>
       </c>
       <c r="E239" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F239" t="s">
         <v>59</v>
@@ -15786,13 +15786,13 @@
         <v>324</v>
       </c>
       <c r="C240" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D240" t="s">
         <v>60</v>
       </c>
       <c r="E240" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F240" t="s">
         <v>59</v>
@@ -15809,13 +15809,13 @@
         <v>325</v>
       </c>
       <c r="C241" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D241" t="s">
         <v>60</v>
       </c>
       <c r="E241" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F241" t="s">
         <v>59</v>
@@ -15832,13 +15832,13 @@
         <v>326</v>
       </c>
       <c r="C242" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D242" t="s">
         <v>60</v>
       </c>
       <c r="E242" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F242" t="s">
         <v>59</v>
@@ -15855,13 +15855,13 @@
         <v>327</v>
       </c>
       <c r="C243" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D243" t="s">
         <v>60</v>
       </c>
       <c r="E243" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F243" t="s">
         <v>59</v>
@@ -15878,13 +15878,13 @@
         <v>328</v>
       </c>
       <c r="C244" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D244" t="s">
         <v>60</v>
       </c>
       <c r="E244" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F244" t="s">
         <v>59</v>
@@ -15901,13 +15901,13 @@
         <v>329</v>
       </c>
       <c r="C245" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D245" t="s">
         <v>60</v>
       </c>
       <c r="E245" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F245" t="s">
         <v>59</v>
@@ -15924,13 +15924,13 @@
         <v>330</v>
       </c>
       <c r="C246" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D246" t="s">
         <v>60</v>
       </c>
       <c r="E246" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F246" t="s">
         <v>59</v>
@@ -15947,13 +15947,13 @@
         <v>331</v>
       </c>
       <c r="C247" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D247" t="s">
         <v>60</v>
       </c>
       <c r="E247" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F247" t="s">
         <v>59</v>
@@ -15970,13 +15970,13 @@
         <v>332</v>
       </c>
       <c r="C248" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D248" t="s">
         <v>60</v>
       </c>
       <c r="E248" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F248" t="s">
         <v>59</v>
@@ -15993,13 +15993,13 @@
         <v>333</v>
       </c>
       <c r="C249" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D249" t="s">
         <v>60</v>
       </c>
       <c r="E249" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F249" t="s">
         <v>59</v>
@@ -16016,13 +16016,13 @@
         <v>334</v>
       </c>
       <c r="C250" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D250" t="s">
         <v>60</v>
       </c>
       <c r="E250" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F250" t="s">
         <v>59</v>
@@ -16039,13 +16039,13 @@
         <v>335</v>
       </c>
       <c r="C251" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D251" t="s">
         <v>60</v>
       </c>
       <c r="E251" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F251" t="s">
         <v>59</v>
@@ -16062,13 +16062,13 @@
         <v>336</v>
       </c>
       <c r="C252" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D252" t="s">
         <v>60</v>
       </c>
       <c r="E252" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F252" t="s">
         <v>59</v>
@@ -16085,13 +16085,13 @@
         <v>337</v>
       </c>
       <c r="C253" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D253" t="s">
         <v>60</v>
       </c>
       <c r="E253" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F253" t="s">
         <v>59</v>
@@ -16108,13 +16108,13 @@
         <v>338</v>
       </c>
       <c r="C254" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D254" t="s">
         <v>60</v>
       </c>
       <c r="E254" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F254" t="s">
         <v>59</v>
@@ -16131,13 +16131,13 @@
         <v>339</v>
       </c>
       <c r="C255" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D255" t="s">
         <v>60</v>
       </c>
       <c r="E255" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F255" t="s">
         <v>59</v>
@@ -16154,13 +16154,13 @@
         <v>340</v>
       </c>
       <c r="C256" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D256" t="s">
         <v>60</v>
       </c>
       <c r="E256" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F256" t="s">
         <v>59</v>
@@ -16177,13 +16177,13 @@
         <v>341</v>
       </c>
       <c r="C257" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D257" t="s">
         <v>60</v>
       </c>
       <c r="E257" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F257" t="s">
         <v>59</v>
@@ -16200,13 +16200,13 @@
         <v>342</v>
       </c>
       <c r="C258" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D258" t="s">
         <v>60</v>
       </c>
       <c r="E258" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F258" t="s">
         <v>59</v>
@@ -16223,13 +16223,13 @@
         <v>343</v>
       </c>
       <c r="C259" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D259" t="s">
         <v>60</v>
       </c>
       <c r="E259" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F259" t="s">
         <v>59</v>
@@ -16246,13 +16246,13 @@
         <v>344</v>
       </c>
       <c r="C260" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D260" t="s">
         <v>60</v>
       </c>
       <c r="E260" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F260" t="s">
         <v>59</v>
@@ -16269,13 +16269,13 @@
         <v>345</v>
       </c>
       <c r="C261" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D261" t="s">
         <v>60</v>
       </c>
       <c r="E261" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F261" t="s">
         <v>59</v>
@@ -16292,13 +16292,13 @@
         <v>346</v>
       </c>
       <c r="C262" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D262" t="s">
         <v>60</v>
       </c>
       <c r="E262" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F262" t="s">
         <v>59</v>
@@ -16315,13 +16315,13 @@
         <v>347</v>
       </c>
       <c r="C263" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D263" t="s">
         <v>60</v>
       </c>
       <c r="E263" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F263" t="s">
         <v>59</v>
@@ -16344,7 +16344,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16429,7 +16429,7 @@
     </row>
     <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="25" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>352</v>

</xml_diff>

<commit_message>
Minor change in mock community total species sum of ctrl2
On branch master
	modified:   recentrifuge/__init__.py
	modified:   recentrifuge/test/TEST.rcf.html
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
	modified:   setup.py
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1380" windowWidth="31460" windowHeight="19500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="22060" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -1700,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J267"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1752,7 +1752,7 @@
         <v>86405</v>
       </c>
       <c r="D2">
-        <v>60381</v>
+        <v>60385</v>
       </c>
       <c r="E2">
         <v>87710</v>
@@ -10231,7 +10231,7 @@
       </c>
       <c r="D267">
         <f t="shared" si="0"/>
-        <v>99996</v>
+        <v>100000</v>
       </c>
       <c r="E267">
         <f t="shared" si="0"/>
@@ -10269,16 +10269,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G263"/>
   <sheetViews>
-    <sheetView topLeftCell="A263" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E263"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="J267" sqref="J267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="54.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10" style="23" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -16344,7 +16346,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update mock and tests after a relevant NCBI Taxonomy change
Former species Asaccharobacter celatus now classified as
Adlercreutzia equolifaciens subsp. celatus (taxid 394340)

On branch master
	modified:   recentrifuge/test/TEST.rcf.html
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijm/local/recentrifuge/recentrifuge/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD8DEA8-CEB0-5A42-BD1C-E95BE05D1AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01391503-EA40-B843-B471-F9E5DA4356A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-8320" windowWidth="68800" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="359">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1110,13 +1113,38 @@
   </si>
   <si>
     <t>Parasphingorhabdus litoris</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Adlercreutzia equolifaciens </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subsp.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> celatus</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1182,6 +1210,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1367,7 +1403,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1423,6 +1459,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1719,9 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J267"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -3201,8 +3236,8 @@
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="1" t="s">
-        <v>129</v>
+      <c r="A47" s="37" t="s">
+        <v>358</v>
       </c>
       <c r="B47">
         <v>394340</v>

</xml_diff>

<commit_message>
Update after NCBI Taxonomy reorganization (Desulfovibrio et al.)
Some Desulfovibrios now Paucidesulfovibrio, Humidesulfovibrio,
Megalodesulfovibrio, or Desulfobaculum.

On branch master
	modified:   README.md
	modified:   recentrifuge/__init__.py
	modified:   recentrifuge/test/TEST.rcf.html
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
	modified:   setup.py
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijm/local/recentrifuge/recentrifuge/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01391503-EA40-B843-B471-F9E5DA4356A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF47011C-CFD3-1D47-8B82-490D51A4D3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-8320" windowWidth="68800" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48540" yWindow="380" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="365">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1138,6 +1138,24 @@
       </rPr>
       <t xml:space="preserve"> celatus</t>
     </r>
+  </si>
+  <si>
+    <t>Pseudodesulfovibrio halophilus</t>
+  </si>
+  <si>
+    <t>Humidesulfovibrio idahonensis</t>
+  </si>
+  <si>
+    <t>Paucidesulfovibrio gracilis</t>
+  </si>
+  <si>
+    <t>Halodesulfovibrio marinisediminis</t>
+  </si>
+  <si>
+    <t>Megalodesulfovibrio paquesii</t>
+  </si>
+  <si>
+    <t>Desulfobaculum senezii</t>
   </si>
 </sst>
 </file>
@@ -1756,7 +1774,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J267"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4901,7 +4921,7 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="1" t="s">
-        <v>181</v>
+        <v>361</v>
       </c>
       <c r="B99">
         <v>47158</v>
@@ -4933,7 +4953,7 @@
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="1" t="s">
-        <v>182</v>
+        <v>359</v>
       </c>
       <c r="B100">
         <v>45629</v>
@@ -4965,7 +4985,7 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="1" t="s">
-        <v>183</v>
+        <v>360</v>
       </c>
       <c r="B101">
         <v>575978</v>
@@ -5029,7 +5049,7 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
-        <v>185</v>
+        <v>362</v>
       </c>
       <c r="B103">
         <v>458711</v>
@@ -5061,7 +5081,7 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="1" t="s">
-        <v>186</v>
+        <v>363</v>
       </c>
       <c r="B104">
         <v>299072</v>
@@ -5093,7 +5113,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="1" t="s">
-        <v>187</v>
+        <v>364</v>
       </c>
       <c r="B105">
         <v>76007</v>

</xml_diff>

<commit_message>
Update after NCBI Taxonomy reorganization (Desulfotomaculum spp.)
Desulfotomaculum spp. now spread in different genera.

On branch master
	modified:   README.md
	modified:   recentrifuge/__init__.py
	modified:   recentrifuge/test/TEST.rcf.html
	modified:   recentrifuge/test/TEST.rcf.xlsx
	modified:   recentrifuge/test/mock.xlsx
	modified:   setup.py
</commit_message>
<xml_diff>
--- a/recentrifuge/test/mock.xlsx
+++ b/recentrifuge/test/mock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijm/local/recentrifuge/recentrifuge/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF47011C-CFD3-1D47-8B82-490D51A4D3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E19177-34ED-F04B-8AAF-B4042D0E598A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48540" yWindow="380" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-42700" yWindow="-2580" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="369">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1156,6 +1156,18 @@
   </si>
   <si>
     <t>Desulfobaculum senezii</t>
+  </si>
+  <si>
+    <t>Desulforamulus aeronauticus</t>
+  </si>
+  <si>
+    <t>Desulfofundulus australicus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desulforamulus putei </t>
+  </si>
+  <si>
+    <t>Desulfofundulus thermosubterraneus</t>
   </si>
 </sst>
 </file>
@@ -1775,7 +1787,7 @@
   <dimension ref="A1:J267"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4761,7 +4773,7 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="1" t="s">
-        <v>176</v>
+        <v>365</v>
       </c>
       <c r="B94">
         <v>53343</v>
@@ -4793,7 +4805,7 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="1" t="s">
-        <v>177</v>
+        <v>366</v>
       </c>
       <c r="B95">
         <v>1566</v>
@@ -4825,7 +4837,7 @@
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="1" t="s">
-        <v>178</v>
+        <v>367</v>
       </c>
       <c r="B96">
         <v>74701</v>
@@ -4857,7 +4869,7 @@
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="1" t="s">
-        <v>179</v>
+        <v>368</v>
       </c>
       <c r="B97">
         <v>348840</v>

</xml_diff>